<commit_message>
correctif IG et statut task c58e430a5ee7bafa5c3e76fac948bf420a9e9a19
</commit_message>
<xml_diff>
--- a/ig/anomalies/StructureDefinition-ror-task.xlsx
+++ b/ig/anomalies/StructureDefinition-ror-task.xlsx
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-12T14:39:26+00:00</t>
+    <t>2023-04-12T15:25:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>